<commit_message>
EFO v3.56.0, DO v2023-07-20
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6831CD56-2946-0F49-B2F6-27896C03CD28}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B470E47-9F20-C046-B64B-D02355DA4CD9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="5220" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Hereditary cancer phenotypes/syndromes</t>
   </si>
   <si>
-    <t>v2023-05-31</t>
-  </si>
-  <si>
     <t>source_description</t>
   </si>
   <si>
@@ -153,10 +150,13 @@
     <t>https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
-    <t>v3.55.1</t>
-  </si>
-  <si>
     <t>medgen</t>
+  </si>
+  <si>
+    <t>v2023-07-20</t>
+  </si>
+  <si>
+    <t>v3.56.0</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,25 +583,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -624,10 +624,10 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -644,16 +644,16 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -670,37 +670,37 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="5"/>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7"/>
     </row>

</xml_diff>

<commit_message>
EFO 3.57, DO 08-08
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B470E47-9F20-C046-B64B-D02355DA4CD9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD4275E-35C6-6846-BF41-76490CE3418B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2023-07-20</t>
-  </si>
-  <si>
-    <t>v3.56.0</t>
+    <t>v2023-08-08</t>
+  </si>
+  <si>
+    <t>v3.57.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
EFO 3.58.0, DO 2023-09-29
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD4275E-35C6-6846-BF41-76490CE3418B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4540655-0F2D-2F47-BBC2-BFD1E99EA5B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2023-08-08</t>
-  </si>
-  <si>
-    <t>v3.57.0</t>
+    <t>v2023-09-29</t>
+  </si>
+  <si>
+    <t>v3.58.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
EFO 3.59, add myelodysplastic syndrome
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4540655-0F2D-2F47-BBC2-BFD1E99EA5B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DB0467-B573-D041-8C0E-8C47DBAC9BF2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <t>v2023-09-29</t>
   </si>
   <si>
-    <t>v3.58.0</t>
+    <t>v3.59.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DO October 2023 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DB0467-B573-D041-8C0E-8C47DBAC9BF2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAEA46A-C0FB-4145-88BB-898035076CF8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2023-09-29</t>
-  </si>
-  <si>
     <t>v3.59.0</t>
+  </si>
+  <si>
+    <t>v2023-10-21</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DO 2023-12, EFO, 2023-12
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAEA46A-C0FB-4145-88BB-898035076CF8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB74AF08-9DBE-7B47-9056-2BE1A6E08933}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.59.0</t>
-  </si>
-  <si>
-    <t>v2023-10-21</t>
+    <t>v3.61.0</t>
+  </si>
+  <si>
+    <t>v2023-12-20</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
EFO update - fix wrong lymph/myelo entries
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB74AF08-9DBE-7B47-9056-2BE1A6E08933}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47169D8-F7E2-6D47-81B6-6FA3EBF8CD03}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.61.0</t>
-  </si>
-  <si>
     <t>v2023-12-20</t>
+  </si>
+  <si>
+    <t>v3.62.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DO january 2024 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47169D8-F7E2-6D47-81B6-6FA3EBF8CD03}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828240E-1172-8B40-8DAB-DF085A77F546}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2023-12-20</t>
-  </si>
-  <si>
     <t>v3.62.0</t>
+  </si>
+  <si>
+    <t>v2024-01-31</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO/DO Feb 2024 update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828240E-1172-8B40-8DAB-DF085A77F546}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B139E2BB-D7EE-4448-AC9E-E88E41F4DBFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.62.0</t>
-  </si>
-  <si>
-    <t>v2024-01-31</t>
+    <t>v3.63.0</t>
+  </si>
+  <si>
+    <t>v2024-02-28</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
DO v2024-03-28, EFO v3.64.0
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B139E2BB-D7EE-4448-AC9E-E88E41F4DBFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA7386-EE58-3546-8CEF-7F772ADAB7AE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="1980" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4500" yWindow="6240" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -156,7 +156,7 @@
     <t>v3.63.0</t>
   </si>
   <si>
-    <t>v2024-02-28</t>
+    <t>v2024-03-28</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DO and EFO updates
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA7386-EE58-3546-8CEF-7F772ADAB7AE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98920D5D-FA4B-EF4A-AA33-D55663DCBD17}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="6240" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.63.0</t>
-  </si>
-  <si>
-    <t>v2024-03-28</t>
+    <t>v2024-04-30</t>
+  </si>
+  <si>
+    <t>v3.65.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO 3.67, DO May 2024
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FE9007-3646-284C-B2D8-AD5C56BED361}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE12162-74D5-7345-B2EA-78B094495962}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2024-04-30</t>
-  </si>
-  <si>
-    <t>v3.66.0</t>
+    <t>v3.67.0</t>
+  </si>
+  <si>
+    <t>v2024-05-29</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DO July 2024 + EFO 3.68 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE12162-74D5-7345-B2EA-78B094495962}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437356D8-F842-B74D-9E22-209D278284A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.67.0</t>
-  </si>
-  <si>
-    <t>v2024-05-29</t>
+    <t>v2024-07-31</t>
+  </si>
+  <si>
+    <t>v3.68.0</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Disease Ontology August 2024 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1485F01-E1D6-9145-B2C4-C6A4978D9BDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715F922C-8996-2748-962C-9DC231960650}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2024-07-31</t>
-  </si>
-  <si>
     <t>v3.69.0</t>
+  </si>
+  <si>
+    <t>v2024-08-29</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO 3.71, DO Sept 2024 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715F922C-8996-2748-962C-9DC231960650}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA3F1D7-B1DE-2E47-89F0-E3A0DF5EE39E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.69.0</t>
-  </si>
-  <si>
-    <t>v2024-08-29</t>
+    <t>v2024-09-27</t>
+  </si>
+  <si>
+    <t>v3.71.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO 3.72, DO 2024-11-01, OncoTree MeSH fix
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA3F1D7-B1DE-2E47-89F0-E3A0DF5EE39E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7369AA46-4F04-5348-99E3-4DDF63CE86C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2024-09-27</t>
-  </si>
-  <si>
-    <t>v3.71.0</t>
+    <t>v2024-11-01</t>
+  </si>
+  <si>
+    <t>v3.72.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
EFO 3.73, DO Dec 2024 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7369AA46-4F04-5348-99E3-4DDF63CE86C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EA753-7E5A-8644-933E-240495783F0A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="5900" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3220" yWindow="2020" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v2024-11-01</t>
-  </si>
-  <si>
-    <t>v3.72.0</t>
+    <t>v3.73.0</t>
+  </si>
+  <si>
+    <t>v2024-12-18</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DO january 2025, EFO 3.74
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EA753-7E5A-8644-933E-240495783F0A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480938AA-1D0F-BA41-BC7C-8822FA0262EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="2020" windowWidth="29560" windowHeight="16500" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.73.0</t>
-  </si>
-  <si>
-    <t>v2024-12-18</t>
+    <t>v2025-02-03</t>
+  </si>
+  <si>
+    <t>v3.74.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
late April DO release
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CA2596-48AA-BF4B-8971-13C499C700ED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0111C-4D98-EC47-82C6-F8D4D4798BCA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="2020" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="920" yWindow="2020" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -153,10 +153,10 @@
     <t>v3.77.0</t>
   </si>
   <si>
-    <t>v2025-03-31</t>
-  </si>
-  <si>
     <t>2025_04_08</t>
+  </si>
+  <si>
+    <t>v2025-04-29</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
EFO and DO update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0111C-4D98-EC47-82C6-F8D4D4798BCA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138479F4-AFED-E84B-A58A-90F545AA8AC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="2020" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
@@ -150,13 +150,13 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.77.0</t>
-  </si>
-  <si>
     <t>2025_04_08</t>
   </si>
   <si>
-    <t>v2025-04-29</t>
+    <t>v3.79.0</t>
+  </si>
+  <si>
+    <t>v2025-06-27</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO 3.80 and DO 2025-08-1
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138479F4-AFED-E84B-A58A-90F545AA8AC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BA06FB-836F-E145-8847-C5CCC53178B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>2025_04_08</t>
   </si>
   <si>
-    <t>v3.79.0</t>
-  </si>
-  <si>
-    <t>v2025-06-27</t>
+    <t>v2025-08-01</t>
+  </si>
+  <si>
+    <t>v3.80.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
EFO 3.83.0, DO Oct 2025
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA9E2A-B896-B54B-8016-6B14DD0A3A40}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE5C71-59D7-BA4F-BD79-2C196859BB38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>2025_04_08</t>
   </si>
   <si>
-    <t>v2025-08-29</t>
-  </si>
-  <si>
-    <t>v3.82.0</t>
+    <t>v3.83.0</t>
+  </si>
+  <si>
+    <t>v2025-10-31</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
OncoTree, DO, EFO updates
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE5C71-59D7-BA4F-BD79-2C196859BB38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD0FB5-83BF-E548-81B3-9BF24A2ADD70}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -150,13 +150,13 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>2025_04_08</t>
-  </si>
-  <si>
-    <t>v3.83.0</t>
-  </si>
-  <si>
-    <t>v2025-10-31</t>
+    <t>v3.84.0</t>
+  </si>
+  <si>
+    <t>v2025-11-25</t>
+  </si>
+  <si>
+    <t>2025_10_03</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032AA6E1-7CD1-0142-A783-7CD36AF8CD61}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DO December release, EFO 3.85.0
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD0FB5-83BF-E548-81B3-9BF24A2ADD70}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD13ADD-1EEB-3947-973A-694081AFA97D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -150,13 +150,13 @@
     <t>medgen</t>
   </si>
   <si>
-    <t>v3.84.0</t>
-  </si>
-  <si>
-    <t>v2025-11-25</t>
-  </si>
-  <si>
     <t>2025_10_03</t>
+  </si>
+  <si>
+    <t>v3.85.0</t>
+  </si>
+  <si>
+    <t>v2025-12-23</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Full OncoTree & EFO 3.87.0
</commit_message>
<xml_diff>
--- a/data-raw/metadata_phen_oncox.xlsx
+++ b/data-raw/metadata_phen_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E33AB8-A05A-284D-8FD8-2A7E78FD983D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4653FA7F-509E-BD42-A2BA-36E6BE26EF94}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="2180" windowWidth="34920" windowHeight="19080" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>2025_10_03</t>
   </si>
   <si>
-    <t>v3.86.0</t>
-  </si>
-  <si>
     <t>v2026-02-02</t>
+  </si>
+  <si>
+    <t>v3.87.0</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>